<commit_message>
Update the data for the Bus30_System
</commit_message>
<xml_diff>
--- a/30_system_data/30-bus 电网干预数据.xlsx
+++ b/30_system_data/30-bus 电网干预数据.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -10,7 +10,7 @@
     <sheet name="branch data" sheetId="1" r:id="rId1"/>
     <sheet name="bus data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -148,8 +148,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,7 +406,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -438,10 +438,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -473,7 +472,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -649,27 +647,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="9" width="9" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="9" style="10" hidden="1" customWidth="1"/>
-    <col min="11" max="12" width="9" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="8.875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="9.25" customWidth="1"/>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="3" max="3" width="12.75" customWidth="1"/>
+    <col min="4" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="9" style="10" customWidth="1"/>
+    <col min="11" max="12" width="9" customWidth="1"/>
+    <col min="13" max="13" width="8.875" customWidth="1"/>
+    <col min="14" max="14" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
         <v>2</v>
       </c>
       <c r="D1">
@@ -694,11 +697,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>3</v>
       </c>
       <c r="D2">
@@ -723,11 +729,14 @@
         <v>2.6833</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16">
       <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>4</v>
       </c>
       <c r="D3">
@@ -752,11 +761,14 @@
         <v>43.890868172438601</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16">
       <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>4</v>
       </c>
       <c r="D4">
@@ -784,11 +796,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16">
       <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>5</v>
       </c>
       <c r="D5">
@@ -813,11 +828,14 @@
         <v>35.158190864789603</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16">
       <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>6</v>
       </c>
       <c r="D6">
@@ -842,11 +860,14 @@
         <v>35.108777778523802</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16">
       <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>6</v>
       </c>
       <c r="D7">
@@ -871,11 +892,14 @@
         <v>31.711950779587099</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16">
       <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>7</v>
       </c>
       <c r="D8">
@@ -900,11 +924,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16">
       <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>7</v>
       </c>
       <c r="D9">
@@ -929,11 +956,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16">
       <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
         <v>6</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>8</v>
       </c>
       <c r="D10">
@@ -958,11 +988,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16">
       <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
         <v>6</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>9</v>
       </c>
       <c r="D11">
@@ -987,11 +1020,14 @@
         <v>21.489894238304199</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16">
       <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
         <v>6</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>10</v>
       </c>
       <c r="D12">
@@ -1016,11 +1052,14 @@
         <v>37.1533034709581</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16">
       <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
         <v>9</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>11</v>
       </c>
       <c r="D13">
@@ -1045,11 +1084,14 @@
         <v>17.0996482487765</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16">
       <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
         <v>9</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>10</v>
       </c>
       <c r="D14">
@@ -1074,11 +1116,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16">
       <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
         <v>4</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>12</v>
       </c>
       <c r="D15">
@@ -1103,11 +1148,14 @@
         <v>21.850241129054901</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16">
       <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
         <v>12</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>13</v>
       </c>
       <c r="D16">
@@ -1132,11 +1180,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:16">
       <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
         <v>12</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>14</v>
       </c>
       <c r="D17">
@@ -1161,11 +1212,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:16">
       <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
         <v>12</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>15</v>
       </c>
       <c r="D18">
@@ -1190,11 +1244,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:16">
       <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
         <v>12</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>16</v>
       </c>
       <c r="D19">
@@ -1219,11 +1276,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:16">
       <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
         <v>14</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>15</v>
       </c>
       <c r="D20">
@@ -1248,11 +1308,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:16">
       <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
         <v>16</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>17</v>
       </c>
       <c r="D21">
@@ -1277,11 +1340,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:16">
       <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
         <v>15</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>18</v>
       </c>
       <c r="D22">
@@ -1306,11 +1372,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:16">
       <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
         <v>18</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>19</v>
       </c>
       <c r="D23">
@@ -1335,11 +1404,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:16">
       <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
         <v>19</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>20</v>
       </c>
       <c r="D24">
@@ -1364,11 +1436,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:16">
       <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
         <v>10</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>20</v>
       </c>
       <c r="D25">
@@ -1393,11 +1468,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:16">
       <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
         <v>10</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>17</v>
       </c>
       <c r="D26">
@@ -1422,11 +1500,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:16">
       <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27">
         <v>10</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>21</v>
       </c>
       <c r="D27">
@@ -1451,11 +1532,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:16">
       <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28">
         <v>10</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>22</v>
       </c>
       <c r="D28">
@@ -1483,11 +1567,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:16">
       <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29">
         <v>21</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>22</v>
       </c>
       <c r="D29">
@@ -1512,11 +1599,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:16">
       <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30">
         <v>15</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>23</v>
       </c>
       <c r="D30">
@@ -1544,11 +1634,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:16">
       <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31">
         <v>22</v>
       </c>
-      <c r="B31">
+      <c r="C31">
         <v>24</v>
       </c>
       <c r="D31">
@@ -1576,11 +1669,14 @@
         <v>12.7807246021501</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:16">
       <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32">
         <v>23</v>
       </c>
-      <c r="B32">
+      <c r="C32">
         <v>24</v>
       </c>
       <c r="D32">
@@ -1605,11 +1701,14 @@
         <v>16.3118816827008</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:16">
       <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33">
         <v>24</v>
       </c>
-      <c r="B33">
+      <c r="C33">
         <v>25</v>
       </c>
       <c r="D33">
@@ -1634,11 +1733,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:16">
       <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34">
         <v>25</v>
       </c>
-      <c r="B34">
+      <c r="C34">
         <v>26</v>
       </c>
       <c r="D34">
@@ -1663,11 +1765,14 @@
         <v>4.2655764313671698</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:16">
       <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35">
         <v>25</v>
       </c>
-      <c r="B35">
+      <c r="C35">
         <v>27</v>
       </c>
       <c r="D35">
@@ -1692,11 +1797,14 @@
         <v>4.2655764313815201</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:16">
       <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36">
         <v>28</v>
       </c>
-      <c r="B36">
+      <c r="C36">
         <v>27</v>
       </c>
       <c r="D36">
@@ -1721,11 +1829,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:16">
       <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37">
         <v>27</v>
       </c>
-      <c r="B37">
+      <c r="C37">
         <v>29</v>
       </c>
       <c r="D37">
@@ -1750,11 +1861,14 @@
         <v>6.3994350255268904</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:16">
       <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38">
         <v>27</v>
       </c>
-      <c r="B38">
+      <c r="C38">
         <v>30</v>
       </c>
       <c r="D38">
@@ -1779,11 +1893,14 @@
         <v>7.3166024082433703</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:16">
       <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39">
         <v>29</v>
       </c>
-      <c r="B39">
+      <c r="C39">
         <v>30</v>
       </c>
       <c r="D39">
@@ -1808,11 +1925,14 @@
         <v>3.7342810122603698</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:16">
       <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40">
         <v>8</v>
       </c>
-      <c r="B40">
+      <c r="C40">
         <v>28</v>
       </c>
       <c r="D40">
@@ -1837,11 +1957,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:16">
       <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41">
         <v>6</v>
       </c>
-      <c r="B41">
+      <c r="C41">
         <v>28</v>
       </c>
       <c r="D41">
@@ -1866,14 +1989,16 @@
         <v>4.64960051236356</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A44" t="s">
+    <row r="42" spans="1:16">
+      <c r="B42" t="s">
         <v>0</v>
       </c>
-      <c r="B44" t="s">
-        <v>1</v>
-      </c>
+      <c r="C42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="14.25" thickBot="1"/>
+    <row r="44" spans="1:16">
       <c r="D44" t="s">
         <v>2</v>
       </c>
@@ -1914,7 +2039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" ht="14.25" thickBot="1">
       <c r="E45" s="14" t="s">
         <v>12</v>
       </c>
@@ -1942,7 +2067,7 @@
       </c>
       <c r="P45" s="19"/>
     </row>
-    <row r="46" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" ht="14.25" thickBot="1">
       <c r="G46" s="14" t="s">
         <v>16</v>
       </c>
@@ -1966,7 +2091,7 @@
       </c>
       <c r="P46" s="19"/>
     </row>
-    <row r="47" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" ht="14.25" thickBot="1">
       <c r="K47" s="14" t="s">
         <v>19</v>
       </c>
@@ -1980,7 +2105,7 @@
       </c>
       <c r="P47" s="19"/>
     </row>
-    <row r="48" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" ht="14.25" thickBot="1">
       <c r="K48" s="4" t="s">
         <v>20</v>
       </c>
@@ -1993,7 +2118,7 @@
       </c>
       <c r="P48" s="19"/>
     </row>
-    <row r="49" spans="11:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="11:16" ht="14.25" thickBot="1">
       <c r="K49" s="4" t="s">
         <v>29</v>
       </c>
@@ -2002,18 +2127,18 @@
       </c>
       <c r="P49" s="15"/>
     </row>
-    <row r="50" spans="11:16" x14ac:dyDescent="0.15">
+    <row r="50" spans="11:16">
       <c r="K50" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="11:16" x14ac:dyDescent="0.15">
+    <row r="51" spans="11:16">
       <c r="K51" s="5" t="s">
         <v>27</v>
       </c>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="11:16" x14ac:dyDescent="0.15">
+    <row r="52" spans="11:16">
       <c r="K52" t="s">
         <v>28</v>
       </c>
@@ -2025,6 +2150,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:C52">
+    <sortCondition ref="A1"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2032,16 +2160,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15">
       <c r="A1">
         <v>1</v>
       </c>
@@ -2067,7 +2195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>2</v>
       </c>
@@ -2093,7 +2221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2119,7 +2247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>4</v>
       </c>
@@ -2145,7 +2273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>5</v>
       </c>
@@ -2171,7 +2299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>6</v>
       </c>
@@ -2197,7 +2325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>7</v>
       </c>
@@ -2223,7 +2351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2249,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15">
       <c r="A9">
         <v>9</v>
       </c>
@@ -2275,7 +2403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15">
       <c r="A10">
         <v>10</v>
       </c>
@@ -2301,7 +2429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15">
       <c r="A11">
         <v>11</v>
       </c>
@@ -2327,7 +2455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15">
       <c r="A12">
         <v>12</v>
       </c>
@@ -2353,7 +2481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15">
       <c r="A13">
         <v>13</v>
       </c>
@@ -2379,7 +2507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15">
       <c r="A14">
         <v>14</v>
       </c>
@@ -2405,7 +2533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15">
       <c r="A15">
         <v>15</v>
       </c>
@@ -2431,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15">
       <c r="A16">
         <v>16</v>
       </c>
@@ -2457,7 +2585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15">
       <c r="A17">
         <v>17</v>
       </c>
@@ -2483,7 +2611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15">
       <c r="A18">
         <v>18</v>
       </c>
@@ -2509,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15">
       <c r="A19">
         <v>19</v>
       </c>
@@ -2535,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15">
       <c r="A20">
         <v>20</v>
       </c>
@@ -2561,7 +2689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15">
       <c r="A21">
         <v>21</v>
       </c>
@@ -2587,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15">
       <c r="A22">
         <v>22</v>
       </c>
@@ -2613,7 +2741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15">
       <c r="A23">
         <v>23</v>
       </c>
@@ -2639,7 +2767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:15">
       <c r="A24">
         <v>24</v>
       </c>
@@ -2665,7 +2793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15">
       <c r="A25">
         <v>25</v>
       </c>
@@ -2691,7 +2819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15">
       <c r="A26">
         <v>26</v>
       </c>
@@ -2717,7 +2845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:15">
       <c r="A27">
         <v>27</v>
       </c>
@@ -2743,7 +2871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15">
       <c r="A28">
         <v>28</v>
       </c>
@@ -2769,7 +2897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15">
       <c r="A29">
         <v>29</v>
       </c>
@@ -2795,7 +2923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15">
       <c r="A30">
         <v>30</v>
       </c>
@@ -2821,7 +2949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.15">
+    <row r="33" spans="3:15">
       <c r="C33" t="s">
         <v>3</v>
       </c>
@@ -2844,17 +2972,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.15">
+    <row r="34" spans="3:15">
       <c r="O34" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.15">
+    <row r="35" spans="3:15">
       <c r="O35" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.15">
+    <row r="36" spans="3:15">
       <c r="G36" t="s">
         <v>14</v>
       </c>
@@ -2862,7 +2990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.15">
+    <row r="37" spans="3:15">
       <c r="O37" s="7" t="s">
         <v>26</v>
       </c>

</xml_diff>